<commit_message>
Cong dien thong tin roi
Cong dien thong tin roi
</commit_message>
<xml_diff>
--- a/Lop NM03.xlsx
+++ b/Lop NM03.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>LỚP NHẬP MÔN 03</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Huỳnh Thị Phương Thủy</t>
+  </si>
+  <si>
+    <t>Le Xuan Cong</t>
   </si>
 </sst>
 </file>
@@ -407,7 +410,7 @@
   <dimension ref="C4:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,6 +452,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>4</v>

</xml_diff>